<commit_message>
add maps for US recodes
</commit_message>
<xml_diff>
--- a/src/covid_historical_model/maps/assay_map.xlsx
+++ b/src/covid_historical_model/maps/assay_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/kt/70vy4dz567xdbx2y3gqtkv800000gp/T/e265a631-9af3-4464-b81c-585cf0712daa/ihme/code/rmbarber/covid-historical-model/src/covid_historical_model/maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C7CCD3-8CBF-0245-8509-0907EDF26B84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3CA635-A050-2C47-871E-7CAF67248076}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20040" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="51">
   <si>
     <t>test_name</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t>N-Roche</t>
+  </si>
+  <si>
+    <t>Abbott ARCHITECT SARS-CoV-2 IgG immunoassay</t>
+  </si>
+  <si>
+    <t>Ortho-Clinical Diagnostics VITROS SARS-CoV-2 IgG immunoassay</t>
+  </si>
+  <si>
+    <t>S-Ortho IgG</t>
   </si>
 </sst>
 </file>
@@ -526,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -569,41 +578,41 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
         <v>42</v>
@@ -611,77 +620,77 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -690,12 +699,12 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -704,127 +713,127 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -835,49 +844,49 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
         <v>16</v>
@@ -891,49 +900,49 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
         <v>9</v>
@@ -947,16 +956,16 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -975,33 +984,64 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D35">
+    <sortCondition ref="A1:A35"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>